<commit_message>
Add serialized Logit model results for financial data analysis
- Introduced a new serialized model file `financesmodel.pkl` containing the fitted Logit model results.
- The model includes parameters related to financial status, CIBIL score, down payment, and undecided finances.
- This addition enables efficient loading and usage of the model for predictions and analysis in future applications.
</commit_message>
<xml_diff>
--- a/BCI backup.xlsx
+++ b/BCI backup.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukulkathuria\Documents\mlprac\driveai\bciindexanalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{40BABC94-642A-4FCE-9F1A-BC5818D23B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93DC8D46-1D06-459A-ACF5-560025425E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="3" xr2:uid="{74E971B4-2156-445C-BAF0-2225205CF2A1}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="536">
   <si>
     <t>Parameters</t>
   </si>
@@ -1433,6 +1433,231 @@
   <si>
     <t>Impact is very high</t>
   </si>
+  <si>
+    <t>Rajiv Mehra</t>
+  </si>
+  <si>
+    <t>Dealer Walk-in</t>
+  </si>
+  <si>
+    <t>Sunita Rao</t>
+  </si>
+  <si>
+    <t>Deepak Shah</t>
+  </si>
+  <si>
+    <t>Ahmedabad</t>
+  </si>
+  <si>
+    <t>8 days</t>
+  </si>
+  <si>
+    <t>Meena Iyer</t>
+  </si>
+  <si>
+    <t>Ramesh Kulkarni</t>
+  </si>
+  <si>
+    <t>11 days</t>
+  </si>
+  <si>
+    <t>Anjali Nair</t>
+  </si>
+  <si>
+    <t>Kochi</t>
+  </si>
+  <si>
+    <t>13 days</t>
+  </si>
+  <si>
+    <t>Vikram Desai</t>
+  </si>
+  <si>
+    <t>9 days</t>
+  </si>
+  <si>
+    <t>Kavita Bansal</t>
+  </si>
+  <si>
+    <t>Jaipur</t>
+  </si>
+  <si>
+    <t>Suresh Menon</t>
+  </si>
+  <si>
+    <t>Thiruvananthapuram</t>
+  </si>
+  <si>
+    <t>Geeta Patil</t>
+  </si>
+  <si>
+    <t>Nagpur</t>
+  </si>
+  <si>
+    <t>L021</t>
+  </si>
+  <si>
+    <t>L022</t>
+  </si>
+  <si>
+    <t>L023</t>
+  </si>
+  <si>
+    <t>L024</t>
+  </si>
+  <si>
+    <t>L025</t>
+  </si>
+  <si>
+    <t>L026</t>
+  </si>
+  <si>
+    <t>L027</t>
+  </si>
+  <si>
+    <t>L028</t>
+  </si>
+  <si>
+    <t>L029</t>
+  </si>
+  <si>
+    <t>L030</t>
+  </si>
+  <si>
+    <t>Neeraj Saxena</t>
+  </si>
+  <si>
+    <t>Lucknow</t>
+  </si>
+  <si>
+    <t>Lata Verma</t>
+  </si>
+  <si>
+    <t>Indore</t>
+  </si>
+  <si>
+    <t>Ajay Khanna</t>
+  </si>
+  <si>
+    <t>Chandigarh</t>
+  </si>
+  <si>
+    <t>Poonam Yadav</t>
+  </si>
+  <si>
+    <t>Bhopal</t>
+  </si>
+  <si>
+    <t>Kiran Deshpande</t>
+  </si>
+  <si>
+    <t>Sneha Rathi</t>
+  </si>
+  <si>
+    <t>Surat</t>
+  </si>
+  <si>
+    <t>Girish Kulkarni</t>
+  </si>
+  <si>
+    <t>Asha Mehta</t>
+  </si>
+  <si>
+    <t>Nikhil Reddy</t>
+  </si>
+  <si>
+    <t>B021</t>
+  </si>
+  <si>
+    <t>Ritu Jain</t>
+  </si>
+  <si>
+    <t>L031</t>
+  </si>
+  <si>
+    <t>L032</t>
+  </si>
+  <si>
+    <t>L033</t>
+  </si>
+  <si>
+    <t>L034</t>
+  </si>
+  <si>
+    <t>L035</t>
+  </si>
+  <si>
+    <t>L036</t>
+  </si>
+  <si>
+    <t>L037</t>
+  </si>
+  <si>
+    <t>L038</t>
+  </si>
+  <si>
+    <t>L039</t>
+  </si>
+  <si>
+    <t>L040</t>
+  </si>
+  <si>
+    <t>B022</t>
+  </si>
+  <si>
+    <t>B023</t>
+  </si>
+  <si>
+    <t>B024</t>
+  </si>
+  <si>
+    <t>B025</t>
+  </si>
+  <si>
+    <t>B026</t>
+  </si>
+  <si>
+    <t>B027</t>
+  </si>
+  <si>
+    <t>B028</t>
+  </si>
+  <si>
+    <t>B029</t>
+  </si>
+  <si>
+    <t>B030</t>
+  </si>
+  <si>
+    <t>B031</t>
+  </si>
+  <si>
+    <t>B032</t>
+  </si>
+  <si>
+    <t>B033</t>
+  </si>
+  <si>
+    <t>B034</t>
+  </si>
+  <si>
+    <t>B035</t>
+  </si>
+  <si>
+    <t>B036</t>
+  </si>
+  <si>
+    <t>B037</t>
+  </si>
+  <si>
+    <t>B038</t>
+  </si>
+  <si>
+    <t>B039</t>
+  </si>
+  <si>
+    <t>B040</t>
+  </si>
 </sst>
 </file>
 
@@ -1443,7 +1668,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1498,6 +1723,12 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Equip Light"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="11">
@@ -1562,7 +1793,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1603,12 +1834,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1713,6 +1962,12 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1737,10 +1992,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -52188,11 +52439,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3EDF3F9-1ED3-45E1-BB66-EC95B7E3C812}">
-  <dimension ref="A1:AD21"/>
+  <dimension ref="A1:AD41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J20" sqref="J20:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52465,7 +52716,7 @@
         <v>271</v>
       </c>
       <c r="S3" s="35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T3" s="35" t="s">
         <v>272</v>
@@ -52486,7 +52737,7 @@
         <v>64</v>
       </c>
       <c r="Z3" s="35">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AA3" s="35" t="s">
         <v>64</v>
@@ -52539,7 +52790,7 @@
         <v>700</v>
       </c>
       <c r="M4" s="36">
-        <v>150000</v>
+        <v>50000</v>
       </c>
       <c r="N4" s="35" t="s">
         <v>15</v>
@@ -52628,7 +52879,7 @@
         <v>287</v>
       </c>
       <c r="L5" s="35">
-        <v>670</v>
+        <v>300</v>
       </c>
       <c r="M5" s="36">
         <v>100000</v>
@@ -52637,7 +52888,7 @@
         <v>15</v>
       </c>
       <c r="O5" s="35" t="s">
-        <v>25</v>
+        <v>229</v>
       </c>
       <c r="P5" s="35" t="s">
         <v>288</v>
@@ -52670,7 +52921,7 @@
         <v>67</v>
       </c>
       <c r="Z5" s="35">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AA5" s="35" t="s">
         <v>64</v>
@@ -52723,7 +52974,7 @@
         <v>850</v>
       </c>
       <c r="M6" s="36">
-        <v>700000</v>
+        <v>70000</v>
       </c>
       <c r="N6" s="35" t="s">
         <v>12</v>
@@ -52741,7 +52992,7 @@
         <v>229</v>
       </c>
       <c r="S6" s="35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="T6" s="35" t="s">
         <v>260</v>
@@ -52854,7 +53105,7 @@
         <v>64</v>
       </c>
       <c r="Z7" s="35">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AA7" s="35" t="s">
         <v>67</v>
@@ -52913,7 +53164,7 @@
         <v>15</v>
       </c>
       <c r="O8" s="35" t="s">
-        <v>25</v>
+        <v>229</v>
       </c>
       <c r="P8" s="35" t="s">
         <v>301</v>
@@ -52946,7 +53197,7 @@
         <v>62</v>
       </c>
       <c r="Z8" s="35">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AA8" s="35" t="s">
         <v>64</v>
@@ -52996,7 +53247,7 @@
         <v>287</v>
       </c>
       <c r="L9" s="35">
-        <v>650</v>
+        <v>450</v>
       </c>
       <c r="M9" s="36">
         <v>50000</v>
@@ -53005,7 +53256,7 @@
         <v>15</v>
       </c>
       <c r="O9" s="35" t="s">
-        <v>25</v>
+        <v>229</v>
       </c>
       <c r="P9" s="35" t="s">
         <v>305</v>
@@ -53174,7 +53425,7 @@
         <v>1400000</v>
       </c>
       <c r="J11" s="35" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K11" s="35" t="s">
         <v>257</v>
@@ -53222,7 +53473,7 @@
         <v>64</v>
       </c>
       <c r="Z11" s="35">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AA11" s="35" t="s">
         <v>64</v>
@@ -53367,13 +53618,13 @@
         <v>720</v>
       </c>
       <c r="M13" s="36">
-        <v>180000</v>
+        <v>80000</v>
       </c>
       <c r="N13" s="35" t="s">
         <v>15</v>
       </c>
       <c r="O13" s="35" t="s">
-        <v>25</v>
+        <v>229</v>
       </c>
       <c r="P13" s="35" t="s">
         <v>258</v>
@@ -53406,7 +53657,7 @@
         <v>62</v>
       </c>
       <c r="Z13" s="35">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AA13" s="35" t="s">
         <v>64</v>
@@ -53450,7 +53701,7 @@
         <v>950000</v>
       </c>
       <c r="J14" s="35" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K14" s="35" t="s">
         <v>269</v>
@@ -53459,7 +53710,7 @@
         <v>780</v>
       </c>
       <c r="M14" s="36">
-        <v>250000</v>
+        <v>50000</v>
       </c>
       <c r="N14" s="35" t="s">
         <v>12</v>
@@ -53557,7 +53808,7 @@
         <v>15</v>
       </c>
       <c r="O15" s="35" t="s">
-        <v>26</v>
+        <v>229</v>
       </c>
       <c r="P15" s="35" t="s">
         <v>311</v>
@@ -53640,10 +53891,10 @@
         <v>269</v>
       </c>
       <c r="L16" s="35">
-        <v>820</v>
+        <v>420</v>
       </c>
       <c r="M16" s="36">
-        <v>400000</v>
+        <v>40000</v>
       </c>
       <c r="N16" s="35" t="s">
         <v>12</v>
@@ -53682,7 +53933,7 @@
         <v>64</v>
       </c>
       <c r="Z16" s="35">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AA16" s="35" t="s">
         <v>64</v>
@@ -53735,13 +53986,13 @@
         <v>710</v>
       </c>
       <c r="M17" s="36">
-        <v>200000</v>
+        <v>20000</v>
       </c>
       <c r="N17" s="35" t="s">
         <v>15</v>
       </c>
       <c r="O17" s="35" t="s">
-        <v>25</v>
+        <v>229</v>
       </c>
       <c r="P17" s="35" t="s">
         <v>331</v>
@@ -53818,16 +54069,16 @@
         <v>850000</v>
       </c>
       <c r="J18" s="35" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K18" s="35" t="s">
         <v>287</v>
       </c>
       <c r="L18" s="35">
-        <v>690</v>
+        <v>600</v>
       </c>
       <c r="M18" s="36">
-        <v>150000</v>
+        <v>70000</v>
       </c>
       <c r="N18" s="35" t="s">
         <v>15</v>
@@ -54094,13 +54345,13 @@
         <v>950000</v>
       </c>
       <c r="J21" s="35" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K21" s="35" t="s">
         <v>287</v>
       </c>
       <c r="L21" s="35">
-        <v>670</v>
+        <v>550</v>
       </c>
       <c r="M21" s="36">
         <v>100000</v>
@@ -54109,7 +54360,7 @@
         <v>15</v>
       </c>
       <c r="O21" s="35" t="s">
-        <v>25</v>
+        <v>229</v>
       </c>
       <c r="P21" s="35" t="s">
         <v>344</v>
@@ -54157,8 +54408,1850 @@
         <v>284</v>
       </c>
     </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" s="35" t="s">
+        <v>481</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>505</v>
+      </c>
+      <c r="C22" s="46" t="s">
+        <v>461</v>
+      </c>
+      <c r="D22" s="46" t="s">
+        <v>462</v>
+      </c>
+      <c r="E22" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="46">
+        <v>45</v>
+      </c>
+      <c r="G22" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="H22" s="46" t="s">
+        <v>279</v>
+      </c>
+      <c r="I22" s="47">
+        <v>1800000</v>
+      </c>
+      <c r="J22" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="K22" s="46" t="s">
+        <v>257</v>
+      </c>
+      <c r="L22" s="46">
+        <v>745</v>
+      </c>
+      <c r="M22" s="46">
+        <v>150000</v>
+      </c>
+      <c r="N22" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="O22" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="P22" s="46" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q22" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="R22" s="46" t="s">
+        <v>374</v>
+      </c>
+      <c r="S22" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T22" s="46" t="s">
+        <v>260</v>
+      </c>
+      <c r="U22" s="46" t="s">
+        <v>260</v>
+      </c>
+      <c r="V22" s="46" t="s">
+        <v>261</v>
+      </c>
+      <c r="W22" s="46" t="s">
+        <v>262</v>
+      </c>
+      <c r="X22" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y22" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z22" s="46">
+        <v>9</v>
+      </c>
+      <c r="AA22" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB22" s="46" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC22" s="46" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD22" s="46" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
+        <v>482</v>
+      </c>
+      <c r="B23" s="35" t="s">
+        <v>517</v>
+      </c>
+      <c r="C23" s="48" t="s">
+        <v>463</v>
+      </c>
+      <c r="D23" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="E23" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" s="48">
+        <v>52</v>
+      </c>
+      <c r="G23" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="48" t="s">
+        <v>268</v>
+      </c>
+      <c r="I23" s="49">
+        <v>1500000</v>
+      </c>
+      <c r="J23" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" s="46" t="s">
+        <v>257</v>
+      </c>
+      <c r="L23" s="48">
+        <v>765</v>
+      </c>
+      <c r="M23" s="48">
+        <v>200000</v>
+      </c>
+      <c r="N23" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O23" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="P23" s="48" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q23" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="R23" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S23" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T23" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U23" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V23" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W23" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X23" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y23" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z23" s="48">
+        <v>10</v>
+      </c>
+      <c r="AA23" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB23" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC23" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD23" s="48" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
+        <v>483</v>
+      </c>
+      <c r="B24" s="35" t="s">
+        <v>518</v>
+      </c>
+      <c r="C24" s="48" t="s">
+        <v>464</v>
+      </c>
+      <c r="D24" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="E24" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F24" s="48">
+        <v>60</v>
+      </c>
+      <c r="G24" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="H24" s="48" t="s">
+        <v>465</v>
+      </c>
+      <c r="I24" s="49">
+        <v>1450000</v>
+      </c>
+      <c r="J24" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" s="46" t="s">
+        <v>257</v>
+      </c>
+      <c r="L24" s="48">
+        <v>735</v>
+      </c>
+      <c r="M24" s="48">
+        <v>180000</v>
+      </c>
+      <c r="N24" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O24" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="P24" s="48" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q24" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="R24" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S24" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T24" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U24" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V24" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W24" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X24" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y24" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z24" s="48">
+        <v>8</v>
+      </c>
+      <c r="AA24" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB24" s="48" t="s">
+        <v>283</v>
+      </c>
+      <c r="AC24" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD24" s="48" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
+        <v>484</v>
+      </c>
+      <c r="B25" s="35" t="s">
+        <v>519</v>
+      </c>
+      <c r="C25" s="48" t="s">
+        <v>467</v>
+      </c>
+      <c r="D25" s="48" t="s">
+        <v>462</v>
+      </c>
+      <c r="E25" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F25" s="48">
+        <v>49</v>
+      </c>
+      <c r="G25" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="48" t="s">
+        <v>292</v>
+      </c>
+      <c r="I25" s="49">
+        <v>1600000</v>
+      </c>
+      <c r="J25" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K25" s="46" t="s">
+        <v>257</v>
+      </c>
+      <c r="L25" s="48">
+        <v>790</v>
+      </c>
+      <c r="M25" s="48">
+        <v>160000</v>
+      </c>
+      <c r="N25" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O25" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="P25" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q25" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="R25" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S25" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T25" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U25" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V25" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W25" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X25" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y25" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z25" s="48">
+        <v>9</v>
+      </c>
+      <c r="AA25" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB25" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC25" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD25" s="48" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A26" s="35" t="s">
+        <v>485</v>
+      </c>
+      <c r="B26" s="35" t="s">
+        <v>520</v>
+      </c>
+      <c r="C26" s="48" t="s">
+        <v>468</v>
+      </c>
+      <c r="D26" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="E26" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="48">
+        <v>55</v>
+      </c>
+      <c r="G26" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="H26" s="48" t="s">
+        <v>286</v>
+      </c>
+      <c r="I26" s="49">
+        <v>1750000</v>
+      </c>
+      <c r="J26" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K26" s="46" t="s">
+        <v>257</v>
+      </c>
+      <c r="L26" s="48">
+        <v>720</v>
+      </c>
+      <c r="M26" s="48">
+        <v>125000</v>
+      </c>
+      <c r="N26" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O26" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="P26" s="48" t="s">
+        <v>469</v>
+      </c>
+      <c r="Q26" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="R26" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S26" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T26" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U26" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V26" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W26" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X26" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y26" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z26" s="48">
+        <v>8</v>
+      </c>
+      <c r="AA26" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB26" s="48" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC26" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD26" s="48" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A27" s="35" t="s">
+        <v>486</v>
+      </c>
+      <c r="B27" s="35" t="s">
+        <v>521</v>
+      </c>
+      <c r="C27" s="48" t="s">
+        <v>470</v>
+      </c>
+      <c r="D27" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="E27" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="48">
+        <v>42</v>
+      </c>
+      <c r="G27" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="48" t="s">
+        <v>471</v>
+      </c>
+      <c r="I27" s="49">
+        <v>1400000</v>
+      </c>
+      <c r="J27" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K27" s="46" t="s">
+        <v>257</v>
+      </c>
+      <c r="L27" s="48">
+        <v>750</v>
+      </c>
+      <c r="M27" s="48">
+        <v>130000</v>
+      </c>
+      <c r="N27" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O27" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="P27" s="48" t="s">
+        <v>472</v>
+      </c>
+      <c r="Q27" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="R27" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S27" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T27" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U27" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V27" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W27" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X27" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y27" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z27" s="48">
+        <v>10</v>
+      </c>
+      <c r="AA27" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB27" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC27" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD27" s="48" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
+        <v>487</v>
+      </c>
+      <c r="B28" s="35" t="s">
+        <v>522</v>
+      </c>
+      <c r="C28" s="48" t="s">
+        <v>473</v>
+      </c>
+      <c r="D28" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="E28" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="48">
+        <v>46</v>
+      </c>
+      <c r="G28" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="H28" s="48" t="s">
+        <v>300</v>
+      </c>
+      <c r="I28" s="49">
+        <v>1900000</v>
+      </c>
+      <c r="J28" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K28" s="46" t="s">
+        <v>257</v>
+      </c>
+      <c r="L28" s="48">
+        <v>770</v>
+      </c>
+      <c r="M28" s="48">
+        <v>140000</v>
+      </c>
+      <c r="N28" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O28" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="P28" s="48" t="s">
+        <v>474</v>
+      </c>
+      <c r="Q28" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="R28" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S28" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T28" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U28" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V28" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W28" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X28" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y28" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z28" s="48">
+        <v>9</v>
+      </c>
+      <c r="AA28" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB28" s="48" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC28" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD28" s="48" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A29" s="35" t="s">
+        <v>488</v>
+      </c>
+      <c r="B29" s="35" t="s">
+        <v>523</v>
+      </c>
+      <c r="C29" s="48" t="s">
+        <v>475</v>
+      </c>
+      <c r="D29" s="48" t="s">
+        <v>462</v>
+      </c>
+      <c r="E29" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="48">
+        <v>53</v>
+      </c>
+      <c r="G29" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="48" t="s">
+        <v>476</v>
+      </c>
+      <c r="I29" s="49">
+        <v>1350000</v>
+      </c>
+      <c r="J29" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K29" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="L29" s="48">
+        <v>725</v>
+      </c>
+      <c r="M29" s="48">
+        <v>175000</v>
+      </c>
+      <c r="N29" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O29" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="P29" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q29" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="R29" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S29" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T29" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U29" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V29" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W29" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X29" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y29" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z29" s="48">
+        <v>8</v>
+      </c>
+      <c r="AA29" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB29" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC29" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD29" s="48" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A30" s="35" t="s">
+        <v>489</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>524</v>
+      </c>
+      <c r="C30" s="48" t="s">
+        <v>477</v>
+      </c>
+      <c r="D30" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="E30" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F30" s="48">
+        <v>65</v>
+      </c>
+      <c r="G30" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="H30" s="48" t="s">
+        <v>478</v>
+      </c>
+      <c r="I30" s="49">
+        <v>1200000</v>
+      </c>
+      <c r="J30" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K30" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="L30" s="48">
+        <v>740</v>
+      </c>
+      <c r="M30" s="48">
+        <v>160000</v>
+      </c>
+      <c r="N30" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O30" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="P30" s="48" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q30" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="R30" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S30" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T30" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U30" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V30" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W30" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X30" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y30" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z30" s="48">
+        <v>10</v>
+      </c>
+      <c r="AA30" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB30" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC30" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD30" s="48" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
+        <v>490</v>
+      </c>
+      <c r="B31" s="35" t="s">
+        <v>525</v>
+      </c>
+      <c r="C31" s="48" t="s">
+        <v>479</v>
+      </c>
+      <c r="D31" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="E31" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" s="48">
+        <v>44</v>
+      </c>
+      <c r="G31" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="48" t="s">
+        <v>480</v>
+      </c>
+      <c r="I31" s="49">
+        <v>1550000</v>
+      </c>
+      <c r="J31" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K31" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="L31" s="48">
+        <v>755</v>
+      </c>
+      <c r="M31" s="48">
+        <v>155000</v>
+      </c>
+      <c r="N31" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O31" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="P31" s="48" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q31" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="R31" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S31" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T31" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U31" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V31" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W31" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X31" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y31" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z31" s="48">
+        <v>9</v>
+      </c>
+      <c r="AA31" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB31" s="48" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC31" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD31" s="48" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
+        <v>507</v>
+      </c>
+      <c r="B32" s="35" t="s">
+        <v>526</v>
+      </c>
+      <c r="C32" s="48" t="s">
+        <v>491</v>
+      </c>
+      <c r="D32" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="E32" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="48">
+        <v>58</v>
+      </c>
+      <c r="G32" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="H32" s="48" t="s">
+        <v>492</v>
+      </c>
+      <c r="I32" s="49">
+        <v>1850000</v>
+      </c>
+      <c r="J32" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K32" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="L32" s="48">
+        <v>760</v>
+      </c>
+      <c r="M32" s="48">
+        <v>170000</v>
+      </c>
+      <c r="N32" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O32" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="P32" s="48" t="s">
+        <v>474</v>
+      </c>
+      <c r="Q32" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="R32" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S32" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T32" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U32" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V32" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W32" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X32" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y32" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z32" s="48">
+        <v>9</v>
+      </c>
+      <c r="AA32" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB32" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC32" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD32" s="48" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
+        <v>508</v>
+      </c>
+      <c r="B33" s="35" t="s">
+        <v>527</v>
+      </c>
+      <c r="C33" s="48" t="s">
+        <v>493</v>
+      </c>
+      <c r="D33" s="48" t="s">
+        <v>462</v>
+      </c>
+      <c r="E33" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="48">
+        <v>47</v>
+      </c>
+      <c r="G33" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="48" t="s">
+        <v>494</v>
+      </c>
+      <c r="I33" s="49">
+        <v>1700000</v>
+      </c>
+      <c r="J33" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K33" s="48" t="s">
+        <v>257</v>
+      </c>
+      <c r="L33" s="48">
+        <v>735</v>
+      </c>
+      <c r="M33" s="48">
+        <v>145000</v>
+      </c>
+      <c r="N33" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O33" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="P33" s="48" t="s">
+        <v>469</v>
+      </c>
+      <c r="Q33" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="R33" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S33" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T33" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U33" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V33" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W33" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X33" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y33" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z33" s="48">
+        <v>8</v>
+      </c>
+      <c r="AA33" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB33" s="48" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC33" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD33" s="48" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A34" s="35" t="s">
+        <v>509</v>
+      </c>
+      <c r="B34" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="C34" s="48" t="s">
+        <v>495</v>
+      </c>
+      <c r="D34" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="E34" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="48">
+        <v>50</v>
+      </c>
+      <c r="G34" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="H34" s="48" t="s">
+        <v>496</v>
+      </c>
+      <c r="I34" s="49">
+        <v>1650000</v>
+      </c>
+      <c r="J34" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K34" s="48" t="s">
+        <v>257</v>
+      </c>
+      <c r="L34" s="48">
+        <v>770</v>
+      </c>
+      <c r="M34" s="48">
+        <v>200000</v>
+      </c>
+      <c r="N34" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O34" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="P34" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q34" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="R34" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S34" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T34" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U34" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V34" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W34" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X34" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y34" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z34" s="48">
+        <v>10</v>
+      </c>
+      <c r="AA34" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB34" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC34" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD34" s="48" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A35" s="35" t="s">
+        <v>510</v>
+      </c>
+      <c r="B35" s="35" t="s">
+        <v>529</v>
+      </c>
+      <c r="C35" s="48" t="s">
+        <v>497</v>
+      </c>
+      <c r="D35" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="E35" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" s="48">
+        <v>56</v>
+      </c>
+      <c r="G35" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="48" t="s">
+        <v>498</v>
+      </c>
+      <c r="I35" s="49">
+        <v>1400000</v>
+      </c>
+      <c r="J35" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K35" s="48" t="s">
+        <v>257</v>
+      </c>
+      <c r="L35" s="48">
+        <v>750</v>
+      </c>
+      <c r="M35" s="48">
+        <v>160000</v>
+      </c>
+      <c r="N35" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O35" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="P35" s="48" t="s">
+        <v>472</v>
+      </c>
+      <c r="Q35" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="R35" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S35" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T35" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U35" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V35" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W35" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X35" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y35" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z35" s="48">
+        <v>8</v>
+      </c>
+      <c r="AA35" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB35" s="48" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC35" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD35" s="48" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A36" s="35" t="s">
+        <v>511</v>
+      </c>
+      <c r="B36" s="35" t="s">
+        <v>530</v>
+      </c>
+      <c r="C36" s="48" t="s">
+        <v>499</v>
+      </c>
+      <c r="D36" s="48" t="s">
+        <v>462</v>
+      </c>
+      <c r="E36" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="48">
+        <v>48</v>
+      </c>
+      <c r="G36" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="H36" s="48" t="s">
+        <v>480</v>
+      </c>
+      <c r="I36" s="49">
+        <v>1300000</v>
+      </c>
+      <c r="J36" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K36" s="48" t="s">
+        <v>257</v>
+      </c>
+      <c r="L36" s="48">
+        <v>740</v>
+      </c>
+      <c r="M36" s="48">
+        <v>180000</v>
+      </c>
+      <c r="N36" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O36" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="P36" s="48" t="s">
+        <v>331</v>
+      </c>
+      <c r="Q36" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="R36" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S36" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T36" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U36" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V36" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W36" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X36" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y36" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z36" s="48">
+        <v>9</v>
+      </c>
+      <c r="AA36" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB36" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC36" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD36" s="48" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A37" s="35" t="s">
+        <v>512</v>
+      </c>
+      <c r="B37" s="35" t="s">
+        <v>531</v>
+      </c>
+      <c r="C37" s="48" t="s">
+        <v>500</v>
+      </c>
+      <c r="D37" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="E37" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F37" s="48">
+        <v>54</v>
+      </c>
+      <c r="G37" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" s="48" t="s">
+        <v>501</v>
+      </c>
+      <c r="I37" s="49">
+        <v>1680000</v>
+      </c>
+      <c r="J37" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K37" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="L37" s="48">
+        <v>725</v>
+      </c>
+      <c r="M37" s="48">
+        <v>130000</v>
+      </c>
+      <c r="N37" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O37" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="P37" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q37" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="R37" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S37" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T37" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U37" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V37" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W37" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X37" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y37" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z37" s="48">
+        <v>8</v>
+      </c>
+      <c r="AA37" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB37" s="48" t="s">
+        <v>283</v>
+      </c>
+      <c r="AC37" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD37" s="48" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A38" s="35" t="s">
+        <v>513</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>532</v>
+      </c>
+      <c r="C38" s="48" t="s">
+        <v>502</v>
+      </c>
+      <c r="D38" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="E38" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F38" s="48">
+        <v>63</v>
+      </c>
+      <c r="G38" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="H38" s="48" t="s">
+        <v>286</v>
+      </c>
+      <c r="I38" s="49">
+        <v>1720000</v>
+      </c>
+      <c r="J38" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K38" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="L38" s="48">
+        <v>755</v>
+      </c>
+      <c r="M38" s="48">
+        <v>150000</v>
+      </c>
+      <c r="N38" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O38" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="P38" s="48" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q38" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="R38" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S38" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T38" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U38" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V38" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W38" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X38" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y38" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z38" s="48">
+        <v>10</v>
+      </c>
+      <c r="AA38" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB38" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC38" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD38" s="48" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A39" s="35" t="s">
+        <v>514</v>
+      </c>
+      <c r="B39" s="35" t="s">
+        <v>533</v>
+      </c>
+      <c r="C39" s="48" t="s">
+        <v>503</v>
+      </c>
+      <c r="D39" s="48" t="s">
+        <v>462</v>
+      </c>
+      <c r="E39" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F39" s="48">
+        <v>46</v>
+      </c>
+      <c r="G39" s="48" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="48" t="s">
+        <v>279</v>
+      </c>
+      <c r="I39" s="49">
+        <v>1530000</v>
+      </c>
+      <c r="J39" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K39" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="L39" s="48">
+        <v>740</v>
+      </c>
+      <c r="M39" s="48">
+        <v>140000</v>
+      </c>
+      <c r="N39" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O39" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="P39" s="48" t="s">
+        <v>466</v>
+      </c>
+      <c r="Q39" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="R39" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S39" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T39" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U39" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V39" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W39" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X39" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y39" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z39" s="48">
+        <v>9</v>
+      </c>
+      <c r="AA39" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB39" s="48" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC39" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD39" s="48" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A40" s="35" t="s">
+        <v>515</v>
+      </c>
+      <c r="B40" s="35" t="s">
+        <v>534</v>
+      </c>
+      <c r="C40" s="48" t="s">
+        <v>504</v>
+      </c>
+      <c r="D40" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="E40" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="F40" s="48">
+        <v>59</v>
+      </c>
+      <c r="G40" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="H40" s="48" t="s">
+        <v>300</v>
+      </c>
+      <c r="I40" s="49">
+        <v>1800000</v>
+      </c>
+      <c r="J40" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="K40" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="L40" s="48">
+        <v>765</v>
+      </c>
+      <c r="M40" s="48">
+        <v>155000</v>
+      </c>
+      <c r="N40" s="48" t="s">
+        <v>12</v>
+      </c>
+      <c r="O40" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="P40" s="48" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q40" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="R40" s="48" t="s">
+        <v>374</v>
+      </c>
+      <c r="S40" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T40" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="U40" s="48" t="s">
+        <v>260</v>
+      </c>
+      <c r="V40" s="48" t="s">
+        <v>261</v>
+      </c>
+      <c r="W40" s="48" t="s">
+        <v>262</v>
+      </c>
+      <c r="X40" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y40" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z40" s="48">
+        <v>9</v>
+      </c>
+      <c r="AA40" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB40" s="48" t="s">
+        <v>263</v>
+      </c>
+      <c r="AC40" s="48" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD40" s="48" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A41" s="35" t="s">
+        <v>516</v>
+      </c>
+      <c r="B41" s="35" t="s">
+        <v>535</v>
+      </c>
+      <c r="C41" s="50" t="s">
+        <v>506</v>
+      </c>
+      <c r="D41" s="50" t="s">
+        <v>209</v>
+      </c>
+      <c r="E41" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" s="50">
+        <v>51</v>
+      </c>
+      <c r="G41" s="50" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" s="50" t="s">
+        <v>476</v>
+      </c>
+      <c r="I41" s="51">
+        <v>1640000</v>
+      </c>
+      <c r="J41" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="K41" s="35" t="s">
+        <v>269</v>
+      </c>
+      <c r="L41" s="50">
+        <v>730</v>
+      </c>
+      <c r="M41" s="50">
+        <v>160000</v>
+      </c>
+      <c r="N41" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="O41" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="P41" s="50" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q41" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="R41" s="50" t="s">
+        <v>374</v>
+      </c>
+      <c r="S41" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="T41" s="50" t="s">
+        <v>260</v>
+      </c>
+      <c r="U41" s="50" t="s">
+        <v>260</v>
+      </c>
+      <c r="V41" s="50" t="s">
+        <v>261</v>
+      </c>
+      <c r="W41" s="50" t="s">
+        <v>262</v>
+      </c>
+      <c r="X41" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y41" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z41" s="50">
+        <v>8</v>
+      </c>
+      <c r="AA41" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB41" s="50" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC41" s="50" t="s">
+        <v>264</v>
+      </c>
+      <c r="AD41" s="50" t="s">
+        <v>265</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -54390,7 +56483,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B1" sqref="B1:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56400,6 +58493,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="531aa0cf-e1ff-42d9-9c91-b573ae12edd2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a346cb88-1c3e-44dc-bfa7-e3e8a752f26d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100133F2EA6F188004CB6B80CD1630D2B26" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1ffd93fd7bc57cd48631ca4ee8ea8635">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="531aa0cf-e1ff-42d9-9c91-b573ae12edd2" xmlns:ns3="a346cb88-1c3e-44dc-bfa7-e3e8a752f26d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8acfe5408f2f40a52e802fb88f4a9837" ns2:_="" ns3:_="">
     <xsd:import namespace="531aa0cf-e1ff-42d9-9c91-b573ae12edd2"/>
@@ -56628,27 +58741,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10DE1BAD-0ED0-4EDF-86A0-2B3C3EC7B3EA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a346cb88-1c3e-44dc-bfa7-e3e8a752f26d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="531aa0cf-e1ff-42d9-9c91-b573ae12edd2"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="531aa0cf-e1ff-42d9-9c91-b573ae12edd2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a346cb88-1c3e-44dc-bfa7-e3e8a752f26d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6103D374-13B4-4689-9302-147D392B6732}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A6111B7-A1EB-475E-9531-B3D8C9B12DA7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -56665,29 +58783,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6103D374-13B4-4689-9302-147D392B6732}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10DE1BAD-0ED0-4EDF-86A0-2B3C3EC7B3EA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a346cb88-1c3e-44dc-bfa7-e3e8a752f26d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="531aa0cf-e1ff-42d9-9c91-b573ae12edd2"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>